<commit_message>
Tested and ran Prateek's functions
</commit_message>
<xml_diff>
--- a/SSW_555/TeamPraRobSud555.xlsx
+++ b/SSW_555/TeamPraRobSud555.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="15960" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="15960" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="198">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -652,9 +652,6 @@
   </si>
   <si>
     <t xml:space="preserve">not started </t>
-  </si>
-  <si>
-    <t>Not Started</t>
   </si>
   <si>
     <t xml:space="preserve">bring alchohol; </t>
@@ -1148,9 +1145,6 @@
               <c:numCache>
                 <c:formatCode>m/d</c:formatCode>
                 <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>41311.0</c:v>
-                </c:pt>
                 <c:pt idx="1">
                   <c:v>41318.0</c:v>
                 </c:pt>
@@ -1169,9 +1163,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
                 <c:pt idx="1">
                   <c:v>42.0</c:v>
                 </c:pt>
@@ -2380,7 +2371,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2483,8 +2474,8 @@
         <v>120</v>
       </c>
       <c r="G16" s="9">
-        <f>(E16-E15)/F16*60</f>
-        <v>125.00000000000001</v>
+        <f>(E16-E15)/F16*G15</f>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.15">
@@ -2573,18 +2564,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11" style="2"/>
     <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="7.1640625" customWidth="1"/>
     <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
@@ -2607,17 +2598,6 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A2" s="2">
-        <v>41311</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
         <v>41318</v>
@@ -2628,6 +2608,9 @@
       <c r="D3">
         <v>143</v>
       </c>
+      <c r="E3">
+        <v>145</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
@@ -2636,8 +2619,18 @@
       <c r="B4">
         <v>37</v>
       </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
       <c r="D4">
         <v>320</v>
+      </c>
+      <c r="E4">
+        <v>300</v>
+      </c>
+      <c r="F4" s="9">
+        <f t="shared" ref="F4:F7" si="0">(D4-D3)/E3*60</f>
+        <v>73.241379310344826</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
@@ -2647,8 +2640,18 @@
       <c r="B5">
         <v>32</v>
       </c>
+      <c r="C5">
+        <v>7.7</v>
+      </c>
       <c r="D5">
-        <v>365</v>
+        <v>370</v>
+      </c>
+      <c r="E5">
+        <v>380</v>
+      </c>
+      <c r="F5" s="9">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -2663,8 +2666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2719,12 +2722,15 @@
         <v>183</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E2">
         <v>25</v>
       </c>
       <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2">
         <v>3</v>
       </c>
       <c r="I2" s="6">
@@ -2741,14 +2747,20 @@
       <c r="C3" s="24" t="s">
         <v>181</v>
       </c>
-      <c r="D3" s="24" t="s">
-        <v>195</v>
+      <c r="D3" s="29" t="s">
+        <v>196</v>
       </c>
       <c r="E3">
         <v>25</v>
       </c>
       <c r="F3">
         <v>3</v>
+      </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
+      <c r="I3" s="6">
+        <v>41334</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
@@ -2762,13 +2774,16 @@
         <v>181</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E4">
         <v>20</v>
       </c>
       <c r="F4">
         <v>2</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
       </c>
       <c r="I4" s="6">
         <v>41329</v>
@@ -2785,7 +2800,7 @@
         <v>182</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E5">
         <v>22</v>
@@ -2814,7 +2829,7 @@
         <v>182</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E6">
         <v>20</v>
@@ -2842,14 +2857,20 @@
       <c r="C7" s="24" t="s">
         <v>181</v>
       </c>
-      <c r="D7" s="24" t="s">
-        <v>195</v>
+      <c r="D7" s="29" t="s">
+        <v>196</v>
       </c>
       <c r="E7">
         <v>20</v>
       </c>
       <c r="F7">
         <v>2</v>
+      </c>
+      <c r="G7">
+        <v>8</v>
+      </c>
+      <c r="I7" s="6">
+        <v>41334</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.15">
@@ -2863,7 +2884,7 @@
         <v>182</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E8">
         <v>15</v>
@@ -2892,12 +2913,15 @@
         <v>183</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E9">
         <v>20</v>
       </c>
       <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
         <v>2</v>
       </c>
       <c r="I9" s="6">
@@ -2915,13 +2939,16 @@
         <v>183</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E10">
         <v>20</v>
       </c>
       <c r="F10">
         <v>2</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
       </c>
       <c r="I10" s="6">
         <v>41332</v>
@@ -2938,13 +2965,16 @@
         <v>183</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E11">
         <v>20</v>
       </c>
       <c r="F11">
         <v>2</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
       </c>
       <c r="I11" s="6">
         <v>41332</v>
@@ -2979,7 +3009,7 @@
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B18" s="28" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.15">
@@ -3054,7 +3084,7 @@
         <v>183</v>
       </c>
       <c r="D2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
@@ -3068,7 +3098,7 @@
         <v>183</v>
       </c>
       <c r="D3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
@@ -3082,7 +3112,7 @@
         <v>181</v>
       </c>
       <c r="D4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="26" x14ac:dyDescent="0.15">
@@ -3096,7 +3126,7 @@
         <v>183</v>
       </c>
       <c r="D5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="26" x14ac:dyDescent="0.15">
@@ -3110,7 +3140,7 @@
         <v>183</v>
       </c>
       <c r="D6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.15">
@@ -3124,7 +3154,7 @@
         <v>181</v>
       </c>
       <c r="D7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="26" x14ac:dyDescent="0.15">
@@ -3138,7 +3168,7 @@
         <v>182</v>
       </c>
       <c r="D8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
@@ -3152,7 +3182,7 @@
         <v>182</v>
       </c>
       <c r="D9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.15">
@@ -3166,7 +3196,7 @@
         <v>182</v>
       </c>
       <c r="D10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="26" x14ac:dyDescent="0.15">
@@ -3180,7 +3210,7 @@
         <v>182</v>
       </c>
       <c r="D11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -3284,7 +3314,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Robert updated xlsx sheet
</commit_message>
<xml_diff>
--- a/SSW_555/TeamPraRobSud555.xlsx
+++ b/SSW_555/TeamPraRobSud555.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17571"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sudhansh/git/SSW_555/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\basilmajdi\Documents\stevens_SSW\agile methods 555\555_proj\SSW555-PatRobSud\SSW_555\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="15960" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="28800" windowHeight="15960" tabRatio="500" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId8"/>
     <sheet name="Stories" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="199">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -661,12 +661,15 @@
   </si>
   <si>
     <t>NOT STARTED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">finished </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -831,7 +834,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -897,6 +900,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -980,7 +984,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1006,22 +1010,22 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>41065.0</c:v>
+                  <c:v>41065</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41078.0</c:v>
+                  <c:v>41078</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41092.0</c:v>
+                  <c:v>41092</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41106.0</c:v>
+                  <c:v>41106</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41120.0</c:v>
+                  <c:v>41120</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1033,25 +1037,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>24.0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-AA0F-472A-8A48-BD2444B41C44}"/>
             </c:ext>
@@ -1077,7 +1081,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1110,14 +1114,14 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1146,13 +1150,13 @@
                 <c:formatCode>m/d</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="1">
-                  <c:v>41318.0</c:v>
+                  <c:v>41318</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41332.0</c:v>
+                  <c:v>41332</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41334.0</c:v>
+                  <c:v>41334</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1164,19 +1168,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="1">
-                  <c:v>42.0</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>37.0</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-17F1-4DF6-AB70-24D0992B24E0}"/>
             </c:ext>
@@ -1235,7 +1239,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1261,7 +1265,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1299,7 +1303,7 @@
         <xdr:cNvPr id="3" name="Rectangular Callout 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1374,7 +1378,7 @@
         <xdr:cNvPr id="4" name="Rectangular Callout 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1439,7 +1443,7 @@
         <xdr:cNvPr id="5" name="Rectangular Callout 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1508,7 +1512,7 @@
         <xdr:cNvPr id="6" name="Rectangular Callout 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1578,7 +1582,7 @@
         <xdr:cNvPr id="7" name="Rectangular Callout 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1647,7 +1651,7 @@
         <xdr:cNvPr id="8" name="Rectangular Callout 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1717,7 +1721,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2064,15 +2068,15 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5" customWidth="1"/>
     <col min="4" max="5" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2089,7 +2093,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>181</v>
       </c>
@@ -2106,7 +2110,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>182</v>
       </c>
@@ -2123,7 +2127,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>183</v>
       </c>
@@ -2140,7 +2144,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D9" s="4" t="s">
         <v>38</v>
       </c>
@@ -2169,16 +2173,16 @@
       <selection activeCell="C2" sqref="C2:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="6.6640625" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.83203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45.83203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.1640625" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.625" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.875" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.875" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.875" style="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.125" style="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B1" s="19" t="s">
         <v>31</v>
       </c>
@@ -2195,7 +2199,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2215,7 +2219,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="24" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" s="24" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2235,7 +2239,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2252,7 +2256,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2269,7 +2273,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2286,7 +2290,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2303,7 +2307,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="32" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2317,7 +2321,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="32" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2331,7 +2335,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2345,7 +2349,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="32" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2374,47 +2378,47 @@
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" style="7"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="3" max="3" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>166</v>
       </c>
@@ -2437,7 +2441,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>167</v>
       </c>
@@ -2453,7 +2457,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>168</v>
       </c>
@@ -2478,7 +2482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>169</v>
       </c>
@@ -2503,7 +2507,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>170</v>
       </c>
@@ -2528,7 +2532,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>171</v>
       </c>
@@ -2568,17 +2572,17 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" style="2"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.625" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="7.125" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="6" max="6" width="13.625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2598,7 +2602,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>41318</v>
       </c>
@@ -2612,7 +2616,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>41332</v>
       </c>
@@ -2629,11 +2633,11 @@
         <v>300</v>
       </c>
       <c r="F4" s="9">
-        <f t="shared" ref="F4:F7" si="0">(D4-D3)/E3*60</f>
+        <f t="shared" ref="F4:F5" si="0">(D4-D3)/E3*60</f>
         <v>73.241379310344826</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>41334</v>
       </c>
@@ -2666,23 +2670,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="1" max="1" width="7.625" customWidth="1"/>
     <col min="2" max="2" width="24.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" customWidth="1"/>
-    <col min="5" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.625" customWidth="1"/>
+    <col min="5" max="5" width="8.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2711,7 +2715,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
         <v>121</v>
       </c>
@@ -2737,7 +2741,7 @@
         <v>41332</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
         <v>130</v>
       </c>
@@ -2763,7 +2767,7 @@
         <v>41334</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>133</v>
       </c>
@@ -2789,7 +2793,7 @@
         <v>41329</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>136</v>
       </c>
@@ -2818,7 +2822,7 @@
         <v>41329</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>140</v>
       </c>
@@ -2847,7 +2851,7 @@
         <v>41322</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>145</v>
       </c>
@@ -2873,7 +2877,7 @@
         <v>41334</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>160</v>
       </c>
@@ -2902,7 +2906,7 @@
         <v>41330</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>119</v>
       </c>
@@ -2928,7 +2932,7 @@
         <v>41332</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>120</v>
       </c>
@@ -2954,7 +2958,7 @@
         <v>41332</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>122</v>
       </c>
@@ -2980,7 +2984,7 @@
         <v>41332</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="26" t="s">
         <v>193</v>
       </c>
@@ -2988,39 +2992,39 @@
         <v>193</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" s="5"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" s="28" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B21" s="28"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B22" s="28"/>
     </row>
   </sheetData>
@@ -3034,17 +3038,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="22.83203125" customWidth="1"/>
-    <col min="4" max="4" width="13.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.875" customWidth="1"/>
+    <col min="4" max="4" width="13.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3073,7 +3077,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="30" t="s">
         <v>123</v>
       </c>
@@ -3084,10 +3088,25 @@
         <v>183</v>
       </c>
       <c r="D2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+        <v>198</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>20</v>
+      </c>
+      <c r="G2">
+        <v>7</v>
+      </c>
+      <c r="H2">
+        <v>15</v>
+      </c>
+      <c r="I2" s="33">
+        <v>41336</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="30" t="s">
         <v>124</v>
       </c>
@@ -3098,10 +3117,25 @@
         <v>183</v>
       </c>
       <c r="D3" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+        <v>198</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>20</v>
+      </c>
+      <c r="G3">
+        <v>7</v>
+      </c>
+      <c r="H3">
+        <v>15</v>
+      </c>
+      <c r="I3" s="33">
+        <v>41336</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="30" t="s">
         <v>125</v>
       </c>
@@ -3114,8 +3148,12 @@
       <c r="D4" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="26" x14ac:dyDescent="0.15">
+      <c r="F4" t="s">
+        <v>193</v>
+      </c>
+      <c r="I4" s="33"/>
+    </row>
+    <row r="5" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="30" t="s">
         <v>126</v>
       </c>
@@ -3126,10 +3164,25 @@
         <v>183</v>
       </c>
       <c r="D5" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="26" x14ac:dyDescent="0.15">
+        <v>198</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+      <c r="F5">
+        <v>20</v>
+      </c>
+      <c r="G5">
+        <v>7</v>
+      </c>
+      <c r="H5">
+        <v>15</v>
+      </c>
+      <c r="I5" s="33">
+        <v>41336</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="30" t="s">
         <v>127</v>
       </c>
@@ -3140,10 +3193,25 @@
         <v>183</v>
       </c>
       <c r="D6" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+        <v>198</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>20</v>
+      </c>
+      <c r="G6">
+        <v>7</v>
+      </c>
+      <c r="H6">
+        <v>15</v>
+      </c>
+      <c r="I6" s="33">
+        <v>41336</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="30" t="s">
         <v>128</v>
       </c>
@@ -3157,7 +3225,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="26" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="30" t="s">
         <v>137</v>
       </c>
@@ -3171,7 +3239,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="30" t="s">
         <v>138</v>
       </c>
@@ -3185,7 +3253,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="30" t="s">
         <v>139</v>
       </c>
@@ -3199,7 +3267,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="26" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A11" s="30" t="s">
         <v>141</v>
       </c>
@@ -3228,9 +3296,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3273,9 +3341,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3318,13 +3386,13 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>118</v>
       </c>
@@ -3335,7 +3403,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>119</v>
       </c>
@@ -3346,7 +3414,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>120</v>
       </c>
@@ -3357,7 +3425,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>121</v>
       </c>
@@ -3368,7 +3436,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>122</v>
       </c>
@@ -3379,7 +3447,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A6" s="30" t="s">
         <v>123</v>
       </c>
@@ -3390,7 +3458,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A7" s="30" t="s">
         <v>124</v>
       </c>
@@ -3401,7 +3469,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="48" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A8" s="30" t="s">
         <v>125</v>
       </c>
@@ -3412,7 +3480,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A9" s="30" t="s">
         <v>126</v>
       </c>
@@ -3423,7 +3491,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A10" s="30" t="s">
         <v>127</v>
       </c>
@@ -3434,7 +3502,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A11" s="30" t="s">
         <v>128</v>
       </c>
@@ -3445,7 +3513,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>129</v>
       </c>
@@ -3456,7 +3524,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="48" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
         <v>130</v>
       </c>
@@ -3467,7 +3535,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="64" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" ht="63" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>131</v>
       </c>
@@ -3478,7 +3546,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>132</v>
       </c>
@@ -3489,7 +3557,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
         <v>133</v>
       </c>
@@ -3500,7 +3568,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>134</v>
       </c>
@@ -3511,7 +3579,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>135</v>
       </c>
@@ -3522,7 +3590,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
         <v>136</v>
       </c>
@@ -3533,7 +3601,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A20" s="30" t="s">
         <v>137</v>
       </c>
@@ -3544,7 +3612,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A21" s="30" t="s">
         <v>138</v>
       </c>
@@ -3555,7 +3623,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A22" s="30" t="s">
         <v>139</v>
       </c>
@@ -3566,7 +3634,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
         <v>140</v>
       </c>
@@ -3577,7 +3645,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A24" s="30" t="s">
         <v>141</v>
       </c>
@@ -3588,7 +3656,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="48" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>142</v>
       </c>
@@ -3599,7 +3667,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>143</v>
       </c>
@@ -3610,7 +3678,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="128" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:3" ht="126" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>144</v>
       </c>
@@ -3621,7 +3689,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
         <v>145</v>
       </c>
@@ -3632,7 +3700,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A29" s="24" t="s">
         <v>146</v>
       </c>
@@ -3643,7 +3711,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>147</v>
       </c>
@@ -3654,7 +3722,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>148</v>
       </c>
@@ -3665,7 +3733,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>149</v>
       </c>
@@ -3676,7 +3744,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>150</v>
       </c>
@@ -3687,7 +3755,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>151</v>
       </c>
@@ -3698,7 +3766,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="48" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>152</v>
       </c>
@@ -3709,7 +3777,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>153</v>
       </c>
@@ -3720,7 +3788,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>154</v>
       </c>
@@ -3731,7 +3799,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>155</v>
       </c>
@@ -3742,7 +3810,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>156</v>
       </c>
@@ -3753,7 +3821,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>157</v>
       </c>
@@ -3764,7 +3832,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>158</v>
       </c>
@@ -3775,7 +3843,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>159</v>
       </c>
@@ -3786,7 +3854,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A43" s="17" t="s">
         <v>160</v>
       </c>

</xml_diff>

<commit_message>
Minor changes to Rob's func, added my story of gender roles
</commit_message>
<xml_diff>
--- a/SSW_555/TeamPraRobSud555.xlsx
+++ b/SSW_555/TeamPraRobSud555.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27907"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\basilmajdi\Documents\stevens_SSW\agile methods 555\555_proj\SSW555-PatRobSud\SSW_555\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sudhansh/git/SSW_555/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="28800" windowHeight="15960" tabRatio="500" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="10000" windowHeight="15960" tabRatio="500" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId8"/>
     <sheet name="Stories" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="200">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -664,12 +664,15 @@
   </si>
   <si>
     <t xml:space="preserve">finished </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finished </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -984,7 +987,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1010,22 +1013,22 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>41065</c:v>
+                  <c:v>41065.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41078</c:v>
+                  <c:v>41078.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41092</c:v>
+                  <c:v>41092.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41106</c:v>
+                  <c:v>41106.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41120</c:v>
+                  <c:v>41120.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1037,25 +1040,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-AA0F-472A-8A48-BD2444B41C44}"/>
             </c:ext>
@@ -1071,28 +1074,28 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1749319312"/>
-        <c:axId val="1749321632"/>
+        <c:axId val="-278290496"/>
+        <c:axId val="-278287296"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="1749319312"/>
+        <c:axId val="-278290496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1749321632"/>
+        <c:crossAx val="-278287296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="1749321632"/>
+        <c:axId val="-278287296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1103,7 +1106,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1749319312"/>
+        <c:crossAx val="-278290496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1114,14 +1117,14 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1150,13 +1153,13 @@
                 <c:formatCode>m/d</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="1">
-                  <c:v>41318</c:v>
+                  <c:v>41318.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41332</c:v>
+                  <c:v>41332.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41334</c:v>
+                  <c:v>41334.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1168,19 +1171,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="1">
-                  <c:v>42</c:v>
+                  <c:v>42.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>37</c:v>
+                  <c:v>37.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-17F1-4DF6-AB70-24D0992B24E0}"/>
             </c:ext>
@@ -1196,11 +1199,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1652432352"/>
-        <c:axId val="1652435104"/>
+        <c:axId val="-279044976"/>
+        <c:axId val="-279042656"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="1652432352"/>
+        <c:axId val="-279044976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1210,14 +1213,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1652435104"/>
+        <c:crossAx val="-279042656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="1652435104"/>
+        <c:axId val="-279042656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1228,7 +1231,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1652432352"/>
+        <c:crossAx val="-279044976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1239,7 +1242,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1265,7 +1268,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1303,7 +1306,7 @@
         <xdr:cNvPr id="3" name="Rectangular Callout 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1378,7 +1381,7 @@
         <xdr:cNvPr id="4" name="Rectangular Callout 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1443,7 +1446,7 @@
         <xdr:cNvPr id="5" name="Rectangular Callout 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1512,7 +1515,7 @@
         <xdr:cNvPr id="6" name="Rectangular Callout 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1582,7 +1585,7 @@
         <xdr:cNvPr id="7" name="Rectangular Callout 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1651,7 +1654,7 @@
         <xdr:cNvPr id="8" name="Rectangular Callout 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1721,7 +1724,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2068,15 +2071,15 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5" customWidth="1"/>
     <col min="4" max="5" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2093,7 +2096,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>181</v>
       </c>
@@ -2110,7 +2113,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>182</v>
       </c>
@@ -2127,7 +2130,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>183</v>
       </c>
@@ -2144,7 +2147,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="D9" s="4" t="s">
         <v>38</v>
       </c>
@@ -2173,16 +2176,16 @@
       <selection activeCell="C2" sqref="C2:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="6.625" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.875" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.875" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45.875" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.125" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.83203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.83203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" style="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="B1" s="19" t="s">
         <v>31</v>
       </c>
@@ -2199,7 +2202,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2219,7 +2222,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="24" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" s="24" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2239,7 +2242,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2256,7 +2259,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2273,7 +2276,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2290,7 +2293,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2307,7 +2310,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="32" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2321,7 +2324,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="32" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2335,7 +2338,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="32" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2349,7 +2352,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="32" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2378,47 +2381,47 @@
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11" style="7"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>166</v>
       </c>
@@ -2441,7 +2444,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>167</v>
       </c>
@@ -2457,7 +2460,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>168</v>
       </c>
@@ -2482,7 +2485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="7" t="s">
         <v>169</v>
       </c>
@@ -2507,7 +2510,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="7" t="s">
         <v>170</v>
       </c>
@@ -2532,7 +2535,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="7" t="s">
         <v>171</v>
       </c>
@@ -2572,17 +2575,17 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11" style="2"/>
-    <col min="2" max="2" width="16.625" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="7.125" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
-    <col min="6" max="6" width="13.625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2602,7 +2605,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
         <v>41318</v>
       </c>
@@ -2616,7 +2619,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
         <v>41332</v>
       </c>
@@ -2637,7 +2640,7 @@
         <v>73.241379310344826</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
         <v>41334</v>
       </c>
@@ -2674,19 +2677,19 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.625" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
     <col min="2" max="2" width="24.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.625" customWidth="1"/>
-    <col min="5" max="5" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2715,7 +2718,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="21" t="s">
         <v>121</v>
       </c>
@@ -2741,7 +2744,7 @@
         <v>41332</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="22" t="s">
         <v>130</v>
       </c>
@@ -2767,7 +2770,7 @@
         <v>41334</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>133</v>
       </c>
@@ -2793,7 +2796,7 @@
         <v>41329</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>136</v>
       </c>
@@ -2822,7 +2825,7 @@
         <v>41329</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>140</v>
       </c>
@@ -2851,7 +2854,7 @@
         <v>41322</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>145</v>
       </c>
@@ -2877,7 +2880,7 @@
         <v>41334</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>160</v>
       </c>
@@ -2906,7 +2909,7 @@
         <v>41330</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>119</v>
       </c>
@@ -2932,7 +2935,7 @@
         <v>41332</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>120</v>
       </c>
@@ -2958,7 +2961,7 @@
         <v>41332</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>122</v>
       </c>
@@ -2984,7 +2987,7 @@
         <v>41332</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" s="26" t="s">
         <v>193</v>
       </c>
@@ -2992,39 +2995,39 @@
         <v>193</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B14" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B15" s="5"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B16" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B17" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B18" s="28" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B20" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B21" s="28"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B22" s="28"/>
     </row>
   </sheetData>
@@ -3038,17 +3041,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="22.875" customWidth="1"/>
-    <col min="4" max="4" width="13.125" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3077,7 +3080,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="30" t="s">
         <v>123</v>
       </c>
@@ -3106,7 +3109,7 @@
         <v>41336</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="30" t="s">
         <v>124</v>
       </c>
@@ -3135,7 +3138,7 @@
         <v>41336</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="30" t="s">
         <v>125</v>
       </c>
@@ -3153,7 +3156,7 @@
       </c>
       <c r="I4" s="33"/>
     </row>
-    <row r="5" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="30" t="s">
         <v>126</v>
       </c>
@@ -3182,7 +3185,7 @@
         <v>41336</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A6" s="30" t="s">
         <v>127</v>
       </c>
@@ -3211,7 +3214,7 @@
         <v>41336</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="30" t="s">
         <v>128</v>
       </c>
@@ -3225,7 +3228,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A8" s="30" t="s">
         <v>137</v>
       </c>
@@ -3239,7 +3242,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="30" t="s">
         <v>138</v>
       </c>
@@ -3253,7 +3256,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="30" t="s">
         <v>139</v>
       </c>
@@ -3264,10 +3267,25 @@
         <v>182</v>
       </c>
       <c r="D10" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>199</v>
+      </c>
+      <c r="E10">
+        <v>10</v>
+      </c>
+      <c r="F10">
+        <v>20</v>
+      </c>
+      <c r="G10">
+        <v>8</v>
+      </c>
+      <c r="H10">
+        <v>10</v>
+      </c>
+      <c r="I10" s="33">
+        <v>41349</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A11" s="30" t="s">
         <v>141</v>
       </c>
@@ -3296,9 +3314,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3341,9 +3359,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3386,13 +3404,13 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>118</v>
       </c>
@@ -3403,7 +3421,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A2" s="17" t="s">
         <v>119</v>
       </c>
@@ -3414,7 +3432,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A3" s="17" t="s">
         <v>120</v>
       </c>
@@ -3425,7 +3443,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A4" s="17" t="s">
         <v>121</v>
       </c>
@@ -3436,7 +3454,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A5" s="17" t="s">
         <v>122</v>
       </c>
@@ -3447,7 +3465,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A6" s="30" t="s">
         <v>123</v>
       </c>
@@ -3458,7 +3476,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A7" s="30" t="s">
         <v>124</v>
       </c>
@@ -3469,7 +3487,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="48" x14ac:dyDescent="0.15">
       <c r="A8" s="30" t="s">
         <v>125</v>
       </c>
@@ -3480,7 +3498,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A9" s="30" t="s">
         <v>126</v>
       </c>
@@ -3491,7 +3509,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A10" s="30" t="s">
         <v>127</v>
       </c>
@@ -3502,7 +3520,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A11" s="30" t="s">
         <v>128</v>
       </c>
@@ -3513,7 +3531,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>129</v>
       </c>
@@ -3524,7 +3542,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="48" x14ac:dyDescent="0.15">
       <c r="A13" s="17" t="s">
         <v>130</v>
       </c>
@@ -3535,7 +3553,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="63" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="64" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>131</v>
       </c>
@@ -3546,7 +3564,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>132</v>
       </c>
@@ -3557,7 +3575,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A16" s="17" t="s">
         <v>133</v>
       </c>
@@ -3568,7 +3586,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>134</v>
       </c>
@@ -3579,7 +3597,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>135</v>
       </c>
@@ -3590,7 +3608,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A19" s="17" t="s">
         <v>136</v>
       </c>
@@ -3601,7 +3619,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A20" s="30" t="s">
         <v>137</v>
       </c>
@@ -3612,7 +3630,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A21" s="30" t="s">
         <v>138</v>
       </c>
@@ -3623,7 +3641,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A22" s="30" t="s">
         <v>139</v>
       </c>
@@ -3634,7 +3652,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A23" s="17" t="s">
         <v>140</v>
       </c>
@@ -3645,7 +3663,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A24" s="30" t="s">
         <v>141</v>
       </c>
@@ -3656,7 +3674,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="48" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>142</v>
       </c>
@@ -3667,7 +3685,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>143</v>
       </c>
@@ -3678,7 +3696,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="126" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="128" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>144</v>
       </c>
@@ -3689,7 +3707,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A28" s="17" t="s">
         <v>145</v>
       </c>
@@ -3700,7 +3718,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A29" s="24" t="s">
         <v>146</v>
       </c>
@@ -3711,7 +3729,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>147</v>
       </c>
@@ -3722,7 +3740,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>148</v>
       </c>
@@ -3733,7 +3751,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>149</v>
       </c>
@@ -3744,7 +3762,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>150</v>
       </c>
@@ -3755,7 +3773,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>151</v>
       </c>
@@ -3766,7 +3784,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="48" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>152</v>
       </c>
@@ -3777,7 +3795,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>153</v>
       </c>
@@ -3788,7 +3806,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>154</v>
       </c>
@@ -3799,7 +3817,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>155</v>
       </c>
@@ -3810,7 +3828,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>156</v>
       </c>
@@ -3821,7 +3839,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>157</v>
       </c>
@@ -3832,7 +3850,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>158</v>
       </c>
@@ -3843,7 +3861,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>159</v>
       </c>
@@ -3854,7 +3872,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A43" s="17" t="s">
         <v>160</v>
       </c>

</xml_diff>

<commit_message>
sprint 2 burndown and everything else
</commit_message>
<xml_diff>
--- a/SSW_555/TeamPraRobSud555.xlsx
+++ b/SSW_555/TeamPraRobSud555.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="38400" windowHeight="19560" tabRatio="500" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="15960" tabRatio="500" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="201">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -660,9 +660,6 @@
     <t>COMPLETED</t>
   </si>
   <si>
-    <t>NOT STARTED</t>
-  </si>
-  <si>
     <t xml:space="preserve">finished </t>
   </si>
   <si>
@@ -670,6 +667,9 @@
   </si>
   <si>
     <t>PUSHED TO NEXT SPRINT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FINIshed </t>
   </si>
 </sst>
 </file>
@@ -1077,11 +1077,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1605445856"/>
-        <c:axId val="-1605443104"/>
+        <c:axId val="-1603627856"/>
+        <c:axId val="-1480080336"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-1605445856"/>
+        <c:axId val="-1603627856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1091,14 +1091,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1605443104"/>
+        <c:crossAx val="-1480080336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-1605443104"/>
+        <c:axId val="-1480080336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1109,7 +1109,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1605445856"/>
+        <c:crossAx val="-1603627856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1170,6 +1170,9 @@
                 <c:pt idx="5">
                   <c:v>41349.0</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>41352.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1194,6 +1197,9 @@
                 <c:pt idx="5">
                   <c:v>27.0</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>26.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1214,11 +1220,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1605431264"/>
-        <c:axId val="-1605428512"/>
+        <c:axId val="-1478820432"/>
+        <c:axId val="-1478817680"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-1605431264"/>
+        <c:axId val="-1478820432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1228,14 +1234,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1605428512"/>
+        <c:crossAx val="-1478817680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-1605428512"/>
+        <c:axId val="-1478817680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1246,7 +1252,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1605431264"/>
+        <c:crossAx val="-1478820432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1283,7 +1289,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1321,7 +1327,7 @@
         <xdr:cNvPr id="3" name="Rectangular Callout 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1396,7 +1402,7 @@
         <xdr:cNvPr id="4" name="Rectangular Callout 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1461,7 +1467,7 @@
         <xdr:cNvPr id="5" name="Rectangular Callout 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1530,7 +1536,7 @@
         <xdr:cNvPr id="6" name="Rectangular Callout 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1600,7 +1606,7 @@
         <xdr:cNvPr id="7" name="Rectangular Callout 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1669,7 +1675,7 @@
         <xdr:cNvPr id="8" name="Rectangular Callout 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1739,7 +1745,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2584,10 +2590,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2651,7 +2657,7 @@
         <v>300</v>
       </c>
       <c r="F4" s="9">
-        <f t="shared" ref="F4:F5" si="0">(D4-D3)/E3*60</f>
+        <f t="shared" ref="F4" si="0">(D4-D3)/E3*60</f>
         <v>73.241379310344826</v>
       </c>
     </row>
@@ -2710,6 +2716,24 @@
       <c r="F7" s="9">
         <f>(D7-D6)/E6*60</f>
         <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A8" s="2">
+        <v>41352</v>
+      </c>
+      <c r="B8">
+        <v>26</v>
+      </c>
+      <c r="D8">
+        <v>390</v>
+      </c>
+      <c r="E8">
+        <v>430</v>
+      </c>
+      <c r="F8" s="9">
+        <f>((D8-D7)/E7)*60</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3092,8 +3116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3142,7 +3166,7 @@
         <v>183</v>
       </c>
       <c r="D2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E2">
         <v>10</v>
@@ -3171,7 +3195,7 @@
         <v>183</v>
       </c>
       <c r="D3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E3">
         <v>10</v>
@@ -3200,12 +3224,23 @@
         <v>181</v>
       </c>
       <c r="D4" t="s">
-        <v>197</v>
-      </c>
-      <c r="F4" t="s">
-        <v>193</v>
-      </c>
-      <c r="I4" s="33"/>
+        <v>200</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
+      <c r="I4" s="33">
+        <v>41352</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="30" t="s">
@@ -3218,7 +3253,7 @@
         <v>183</v>
       </c>
       <c r="D5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E5">
         <v>10</v>
@@ -3247,7 +3282,7 @@
         <v>183</v>
       </c>
       <c r="D6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E6">
         <v>10</v>
@@ -3276,7 +3311,7 @@
         <v>181</v>
       </c>
       <c r="D7" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="26" x14ac:dyDescent="0.15">
@@ -3290,7 +3325,7 @@
         <v>182</v>
       </c>
       <c r="D8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
@@ -3304,7 +3339,7 @@
         <v>182</v>
       </c>
       <c r="D9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.15">
@@ -3318,7 +3353,7 @@
         <v>182</v>
       </c>
       <c r="D10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E10">
         <v>10</v>
@@ -3347,7 +3382,7 @@
         <v>182</v>
       </c>
       <c r="D11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed gedcom for sprint 1 and sprint 2 stories
</commit_message>
<xml_diff>
--- a/SSW_555/TeamPraRobSud555.xlsx
+++ b/SSW_555/TeamPraRobSud555.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="15960" tabRatio="500" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="29600" windowHeight="10580" tabRatio="500" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="201">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -840,7 +840,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -907,6 +907,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1077,11 +1080,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1603627856"/>
-        <c:axId val="-1480080336"/>
+        <c:axId val="328008800"/>
+        <c:axId val="328012880"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-1603627856"/>
+        <c:axId val="328008800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1091,14 +1094,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1480080336"/>
+        <c:crossAx val="328012880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-1480080336"/>
+        <c:axId val="328012880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1109,7 +1112,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1603627856"/>
+        <c:crossAx val="328008800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1220,11 +1223,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1478820432"/>
-        <c:axId val="-1478817680"/>
+        <c:axId val="328051392"/>
+        <c:axId val="328054144"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-1478820432"/>
+        <c:axId val="328051392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1234,14 +1237,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1478817680"/>
+        <c:crossAx val="328054144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-1478817680"/>
+        <c:axId val="328054144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1252,7 +1255,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1478820432"/>
+        <c:crossAx val="328051392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1289,7 +1292,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1327,7 +1330,7 @@
         <xdr:cNvPr id="3" name="Rectangular Callout 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1402,7 +1405,7 @@
         <xdr:cNvPr id="4" name="Rectangular Callout 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1467,7 +1470,7 @@
         <xdr:cNvPr id="5" name="Rectangular Callout 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1536,7 +1539,7 @@
         <xdr:cNvPr id="6" name="Rectangular Callout 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1606,7 +1609,7 @@
         <xdr:cNvPr id="7" name="Rectangular Callout 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1675,7 +1678,7 @@
         <xdr:cNvPr id="8" name="Rectangular Callout 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1745,7 +1748,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2749,7 +2752,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2794,7 +2797,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="34" t="s">
         <v>121</v>
       </c>
       <c r="B2" s="21" t="s">
@@ -2820,7 +2823,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="34" t="s">
         <v>130</v>
       </c>
       <c r="B3" s="22" t="s">
@@ -2846,7 +2849,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
+      <c r="A4" s="17" t="s">
         <v>133</v>
       </c>
       <c r="B4" t="s">
@@ -2872,7 +2875,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A5" t="s">
+      <c r="A5" s="17" t="s">
         <v>136</v>
       </c>
       <c r="B5" t="s">
@@ -2901,7 +2904,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
+      <c r="A6" s="17" t="s">
         <v>140</v>
       </c>
       <c r="B6" t="s">
@@ -2930,7 +2933,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A7" t="s">
+      <c r="A7" s="17" t="s">
         <v>145</v>
       </c>
       <c r="B7" t="s">
@@ -2956,7 +2959,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A8" t="s">
+      <c r="A8" s="17" t="s">
         <v>160</v>
       </c>
       <c r="B8" t="s">
@@ -2985,7 +2988,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A9" t="s">
+      <c r="A9" s="17" t="s">
         <v>119</v>
       </c>
       <c r="B9" t="s">
@@ -3011,7 +3014,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A10" t="s">
+      <c r="A10" s="17" t="s">
         <v>120</v>
       </c>
       <c r="B10" t="s">
@@ -3037,7 +3040,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A11" t="s">
+      <c r="A11" s="17" t="s">
         <v>122</v>
       </c>
       <c r="B11" t="s">
@@ -3116,8 +3119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="A5" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3156,7 +3159,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="17" t="s">
         <v>123</v>
       </c>
       <c r="B2" s="32" t="s">
@@ -3185,7 +3188,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="17" t="s">
         <v>124</v>
       </c>
       <c r="B3" s="32" t="s">
@@ -3214,7 +3217,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="17" t="s">
         <v>125</v>
       </c>
       <c r="B4" s="32" t="s">
@@ -3243,7 +3246,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="26" x14ac:dyDescent="0.15">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="17" t="s">
         <v>126</v>
       </c>
       <c r="B5" s="32" t="s">
@@ -3272,7 +3275,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="26" x14ac:dyDescent="0.15">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="17" t="s">
         <v>127</v>
       </c>
       <c r="B6" s="32" t="s">
@@ -3343,7 +3346,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="17" t="s">
         <v>139</v>
       </c>
       <c r="B10" s="32" t="s">
@@ -3394,10 +3397,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3429,6 +3432,50 @@
       </c>
       <c r="I1" s="10" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="26" x14ac:dyDescent="0.15">
+      <c r="A2" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="52" x14ac:dyDescent="0.15">
+      <c r="A3" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="26" x14ac:dyDescent="0.15">
+      <c r="A4" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="39" x14ac:dyDescent="0.15">
+      <c r="A5" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added my sprint 3 story lengths etc
</commit_message>
<xml_diff>
--- a/SSW_555/TeamPraRobSud555.xlsx
+++ b/SSW_555/TeamPraRobSud555.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27907"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\basilmajdi\Documents\stevens_SSW\agile methods 555\555_proj\SSW555-PatRobSud\SSW_555\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sudhansh/git/SSW_555/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="29595" windowHeight="10575" tabRatio="500" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="15960" tabRatio="500" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId8"/>
     <sheet name="Stories" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="203">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -670,12 +670,18 @@
   </si>
   <si>
     <t xml:space="preserve">FINIshed </t>
+  </si>
+  <si>
+    <t>NOT STARTED</t>
+  </si>
+  <si>
+    <t>STARTED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -840,7 +846,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -910,12 +916,22 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -999,7 +1015,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1025,22 +1041,22 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>41065</c:v>
+                  <c:v>41065.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41078</c:v>
+                  <c:v>41078.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41092</c:v>
+                  <c:v>41092.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41106</c:v>
+                  <c:v>41106.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41120</c:v>
+                  <c:v>41120.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1052,25 +1068,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-AA0F-472A-8A48-BD2444B41C44}"/>
             </c:ext>
@@ -1086,28 +1102,28 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="328008800"/>
-        <c:axId val="328012880"/>
+        <c:axId val="1746044288"/>
+        <c:axId val="1746045648"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="328008800"/>
+        <c:axId val="1746044288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="328012880"/>
+        <c:crossAx val="1746045648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="328012880"/>
+        <c:axId val="1746045648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1118,7 +1134,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="328008800"/>
+        <c:crossAx val="1746044288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1129,14 +1145,14 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1165,22 +1181,22 @@
                 <c:formatCode>m/d</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="1">
-                  <c:v>41318</c:v>
+                  <c:v>41318.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41332</c:v>
+                  <c:v>41332.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41334</c:v>
+                  <c:v>41334.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41336</c:v>
+                  <c:v>41336.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>41349</c:v>
+                  <c:v>41349.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>41352</c:v>
+                  <c:v>41352.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1192,28 +1208,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="1">
-                  <c:v>42</c:v>
+                  <c:v>42.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>37</c:v>
+                  <c:v>37.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28</c:v>
+                  <c:v>28.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>27</c:v>
+                  <c:v>27.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>26</c:v>
+                  <c:v>26.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-17F1-4DF6-AB70-24D0992B24E0}"/>
             </c:ext>
@@ -1229,11 +1245,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="328051392"/>
-        <c:axId val="328054144"/>
+        <c:axId val="1745986992"/>
+        <c:axId val="1745989312"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="328051392"/>
+        <c:axId val="1745986992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1243,14 +1259,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="328054144"/>
+        <c:crossAx val="1745989312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="328054144"/>
+        <c:axId val="1745989312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1261,7 +1277,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="328051392"/>
+        <c:crossAx val="1745986992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1272,7 +1288,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1298,7 +1314,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1336,7 +1352,7 @@
         <xdr:cNvPr id="3" name="Rectangular Callout 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1411,7 +1427,7 @@
         <xdr:cNvPr id="4" name="Rectangular Callout 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1476,7 +1492,7 @@
         <xdr:cNvPr id="5" name="Rectangular Callout 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1545,7 +1561,7 @@
         <xdr:cNvPr id="6" name="Rectangular Callout 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1615,7 +1631,7 @@
         <xdr:cNvPr id="7" name="Rectangular Callout 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1684,7 +1700,7 @@
         <xdr:cNvPr id="8" name="Rectangular Callout 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1754,7 +1770,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2101,15 +2117,15 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5" customWidth="1"/>
     <col min="4" max="5" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2126,7 +2142,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>181</v>
       </c>
@@ -2143,7 +2159,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>182</v>
       </c>
@@ -2160,7 +2176,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>183</v>
       </c>
@@ -2177,7 +2193,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="D9" s="4" t="s">
         <v>38</v>
       </c>
@@ -2206,16 +2222,16 @@
       <selection activeCell="C2" sqref="C2:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="6.625" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.875" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.875" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45.875" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.125" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.83203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.83203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" style="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="B1" s="19" t="s">
         <v>31</v>
       </c>
@@ -2232,7 +2248,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2252,7 +2268,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="24" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" s="24" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2272,7 +2288,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2289,7 +2305,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2306,7 +2322,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2323,7 +2339,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2340,7 +2356,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="32" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2354,7 +2370,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="32" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2368,7 +2384,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="32" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2382,7 +2398,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="32" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2411,47 +2427,47 @@
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11" style="7"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>166</v>
       </c>
@@ -2474,7 +2490,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>167</v>
       </c>
@@ -2490,7 +2506,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>168</v>
       </c>
@@ -2515,7 +2531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="7" t="s">
         <v>169</v>
       </c>
@@ -2540,7 +2556,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="7" t="s">
         <v>170</v>
       </c>
@@ -2565,7 +2581,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="7" t="s">
         <v>171</v>
       </c>
@@ -2605,17 +2621,17 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11" style="2"/>
-    <col min="2" max="2" width="16.625" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="7.125" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
-    <col min="6" max="6" width="13.625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2635,7 +2651,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
         <v>41318</v>
       </c>
@@ -2649,7 +2665,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
         <v>41332</v>
       </c>
@@ -2670,7 +2686,7 @@
         <v>73.241379310344826</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
         <v>41334</v>
       </c>
@@ -2691,7 +2707,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
         <v>41336</v>
       </c>
@@ -2709,7 +2725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
         <v>41349</v>
       </c>
@@ -2727,7 +2743,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" s="2">
         <v>41352</v>
       </c>
@@ -2761,19 +2777,19 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.625" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
     <col min="2" max="2" width="24.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.625" customWidth="1"/>
-    <col min="5" max="5" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2802,7 +2818,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="34" t="s">
         <v>121</v>
       </c>
@@ -2828,7 +2844,7 @@
         <v>41332</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="34" t="s">
         <v>130</v>
       </c>
@@ -2854,7 +2870,7 @@
         <v>41334</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="17" t="s">
         <v>133</v>
       </c>
@@ -2880,7 +2896,7 @@
         <v>41329</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="17" t="s">
         <v>136</v>
       </c>
@@ -2909,7 +2925,7 @@
         <v>41329</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="17" t="s">
         <v>140</v>
       </c>
@@ -2938,7 +2954,7 @@
         <v>41322</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="17" t="s">
         <v>145</v>
       </c>
@@ -2964,7 +2980,7 @@
         <v>41334</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="17" t="s">
         <v>160</v>
       </c>
@@ -2993,7 +3009,7 @@
         <v>41330</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="17" t="s">
         <v>119</v>
       </c>
@@ -3019,7 +3035,7 @@
         <v>41332</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="17" t="s">
         <v>120</v>
       </c>
@@ -3045,7 +3061,7 @@
         <v>41332</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" s="17" t="s">
         <v>122</v>
       </c>
@@ -3071,7 +3087,7 @@
         <v>41332</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" s="26" t="s">
         <v>193</v>
       </c>
@@ -3079,39 +3095,39 @@
         <v>193</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B14" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B15" s="5"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B16" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B17" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B18" s="28" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B20" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B21" s="28"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B22" s="28"/>
     </row>
   </sheetData>
@@ -3125,17 +3141,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="A11" sqref="A11:C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="22.875" customWidth="1"/>
-    <col min="4" max="4" width="13.125" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3164,7 +3180,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="17" t="s">
         <v>123</v>
       </c>
@@ -3193,7 +3209,7 @@
         <v>41336</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="17" t="s">
         <v>124</v>
       </c>
@@ -3222,7 +3238,7 @@
         <v>41336</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="17" t="s">
         <v>125</v>
       </c>
@@ -3251,7 +3267,7 @@
         <v>41352</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="17" t="s">
         <v>126</v>
       </c>
@@ -3280,7 +3296,7 @@
         <v>41336</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A6" s="17" t="s">
         <v>127</v>
       </c>
@@ -3309,7 +3325,7 @@
         <v>41336</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="30" t="s">
         <v>128</v>
       </c>
@@ -3323,7 +3339,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A8" s="30" t="s">
         <v>137</v>
       </c>
@@ -3337,7 +3353,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="30" t="s">
         <v>138</v>
       </c>
@@ -3351,7 +3367,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="17" t="s">
         <v>139</v>
       </c>
@@ -3380,7 +3396,7 @@
         <v>41349</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A11" s="30" t="s">
         <v>141</v>
       </c>
@@ -3406,131 +3422,199 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="24.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.125" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.1640625" style="35" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.15">
+      <c r="A1" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="38" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="30" t="s">
+    <row r="2" spans="1:9" ht="26" x14ac:dyDescent="0.15">
+      <c r="A2" s="37" t="s">
         <v>128</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="39" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A3" s="30" t="s">
+      <c r="D2" s="39" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+    </row>
+    <row r="3" spans="1:9" ht="26" x14ac:dyDescent="0.15">
+      <c r="A3" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="39" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="30" t="s">
+      <c r="D3" s="39" t="s">
+        <v>202</v>
+      </c>
+      <c r="E3" s="39">
+        <v>15</v>
+      </c>
+      <c r="F3" s="39">
+        <v>6</v>
+      </c>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A4" s="37" t="s">
         <v>138</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="37" t="s">
         <v>92</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="39" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="30" t="s">
+      <c r="D4" s="39" t="s">
+        <v>202</v>
+      </c>
+      <c r="E4" s="39">
+        <v>15</v>
+      </c>
+      <c r="F4" s="39">
+        <v>6</v>
+      </c>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+    </row>
+    <row r="5" spans="1:9" ht="26" x14ac:dyDescent="0.15">
+      <c r="A5" s="37" t="s">
         <v>141</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="39" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="D5" s="39" t="s">
+        <v>201</v>
+      </c>
+      <c r="E5" s="39">
+        <v>20</v>
+      </c>
+      <c r="F5" s="39">
+        <v>7</v>
+      </c>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+    </row>
+    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+      <c r="A6" s="39" t="s">
         <v>153</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="20" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
+    </row>
+    <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+      <c r="A7" s="39" t="s">
         <v>154</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="C7" s="20" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A8" s="39" t="s">
         <v>156</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="39" t="s">
         <v>111</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="40" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A9" s="39" t="s">
         <v>157</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="40" t="s">
         <v>183</v>
       </c>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -3547,9 +3631,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3592,13 +3676,13 @@
       <selection activeCell="A40" sqref="A39:B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>118</v>
       </c>
@@ -3609,7 +3693,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A2" s="17" t="s">
         <v>119</v>
       </c>
@@ -3620,7 +3704,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A3" s="17" t="s">
         <v>120</v>
       </c>
@@ -3631,7 +3715,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A4" s="17" t="s">
         <v>121</v>
       </c>
@@ -3642,7 +3726,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A5" s="17" t="s">
         <v>122</v>
       </c>
@@ -3653,7 +3737,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A6" s="30" t="s">
         <v>123</v>
       </c>
@@ -3664,7 +3748,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A7" s="30" t="s">
         <v>124</v>
       </c>
@@ -3675,7 +3759,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="48" x14ac:dyDescent="0.15">
       <c r="A8" s="30" t="s">
         <v>125</v>
       </c>
@@ -3686,7 +3770,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A9" s="30" t="s">
         <v>126</v>
       </c>
@@ -3697,7 +3781,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A10" s="30" t="s">
         <v>127</v>
       </c>
@@ -3708,7 +3792,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A11" s="30" t="s">
         <v>128</v>
       </c>
@@ -3719,7 +3803,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>129</v>
       </c>
@@ -3730,7 +3814,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="48" x14ac:dyDescent="0.15">
       <c r="A13" s="17" t="s">
         <v>130</v>
       </c>
@@ -3741,7 +3825,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="63" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="64" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>131</v>
       </c>
@@ -3752,7 +3836,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>132</v>
       </c>
@@ -3763,7 +3847,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A16" s="17" t="s">
         <v>133</v>
       </c>
@@ -3774,7 +3858,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>134</v>
       </c>
@@ -3785,7 +3869,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>135</v>
       </c>
@@ -3796,7 +3880,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A19" s="17" t="s">
         <v>136</v>
       </c>
@@ -3807,7 +3891,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A20" s="30" t="s">
         <v>137</v>
       </c>
@@ -3818,7 +3902,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A21" s="30" t="s">
         <v>138</v>
       </c>
@@ -3829,7 +3913,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A22" s="30" t="s">
         <v>139</v>
       </c>
@@ -3840,7 +3924,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A23" s="17" t="s">
         <v>140</v>
       </c>
@@ -3851,7 +3935,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A24" s="30" t="s">
         <v>141</v>
       </c>
@@ -3862,7 +3946,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="48" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>142</v>
       </c>
@@ -3873,7 +3957,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>143</v>
       </c>
@@ -3884,7 +3968,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="126" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="128" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>144</v>
       </c>
@@ -3895,7 +3979,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A28" s="17" t="s">
         <v>145</v>
       </c>
@@ -3906,7 +3990,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A29" s="24" t="s">
         <v>146</v>
       </c>
@@ -3917,7 +4001,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>147</v>
       </c>
@@ -3928,7 +4012,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>148</v>
       </c>
@@ -3939,7 +4023,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>149</v>
       </c>
@@ -3950,7 +4034,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>150</v>
       </c>
@@ -3961,7 +4045,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>151</v>
       </c>
@@ -3972,7 +4056,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="48" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>152</v>
       </c>
@@ -3983,7 +4067,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>153</v>
       </c>
@@ -3994,7 +4078,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>154</v>
       </c>
@@ -4005,7 +4089,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>155</v>
       </c>
@@ -4016,7 +4100,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>156</v>
       </c>
@@ -4027,7 +4111,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>157</v>
       </c>
@@ -4038,7 +4122,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>158</v>
       </c>
@@ -4049,7 +4133,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>159</v>
       </c>
@@ -4060,7 +4144,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A43" s="17" t="s">
         <v>160</v>
       </c>

</xml_diff>

<commit_message>
Updated sprint 3 (my work) and burndown
</commit_message>
<xml_diff>
--- a/SSW_555/TeamPraRobSud555.xlsx
+++ b/SSW_555/TeamPraRobSud555.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10820" yWindow="440" windowWidth="17980" windowHeight="15960" tabRatio="500" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="15960" tabRatio="500" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -1166,11 +1166,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1462338144"/>
-        <c:axId val="-1462334736"/>
+        <c:axId val="-1323814192"/>
+        <c:axId val="-1323811872"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-1462338144"/>
+        <c:axId val="-1323814192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1180,14 +1180,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1462334736"/>
+        <c:crossAx val="-1323811872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-1462334736"/>
+        <c:axId val="-1323811872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1198,7 +1198,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1462338144"/>
+        <c:crossAx val="-1323814192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1293,7 +1293,7 @@
                   <c:v>26.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>24.0</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1315,11 +1315,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1360531088"/>
-        <c:axId val="-1360528336"/>
+        <c:axId val="-1343928656"/>
+        <c:axId val="-1343981120"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-1360531088"/>
+        <c:axId val="-1343928656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1329,14 +1329,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1360528336"/>
+        <c:crossAx val="-1343981120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-1360528336"/>
+        <c:axId val="-1343981120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1347,7 +1347,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1360531088"/>
+        <c:crossAx val="-1343928656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1384,7 +1384,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1422,7 +1422,7 @@
         <xdr:cNvPr id="3" name="Rectangular Callout 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1497,7 +1497,7 @@
         <xdr:cNvPr id="4" name="Rectangular Callout 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1562,7 +1562,7 @@
         <xdr:cNvPr id="5" name="Rectangular Callout 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1631,7 +1631,7 @@
         <xdr:cNvPr id="6" name="Rectangular Callout 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1701,7 +1701,7 @@
         <xdr:cNvPr id="7" name="Rectangular Callout 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1770,7 +1770,7 @@
         <xdr:cNvPr id="8" name="Rectangular Callout 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1840,7 +1840,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2687,8 +2687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2836,17 +2836,17 @@
         <v>41364</v>
       </c>
       <c r="B9">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D9">
-        <v>425</v>
+        <v>437</v>
       </c>
       <c r="E9">
-        <v>500</v>
+        <v>520</v>
       </c>
       <c r="F9" s="9">
         <f>((D9-D8)/E8)*60</f>
-        <v>4.8837209302325588</v>
+        <v>6.558139534883721</v>
       </c>
     </row>
   </sheetData>
@@ -3540,8 +3540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="C2" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3630,7 +3630,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="44" t="s">
         <v>135</v>
       </c>
       <c r="B4" s="35" t="s">
@@ -3658,7 +3658,7 @@
         <v>41364</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="26" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="35" t="s">
         <v>138</v>
       </c>
@@ -3669,7 +3669,7 @@
         <v>179</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="E5" s="37">
         <v>20</v>
@@ -3677,9 +3677,15 @@
       <c r="F5" s="37">
         <v>7</v>
       </c>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
+      <c r="G5" s="37">
+        <v>12</v>
+      </c>
+      <c r="H5" s="37">
+        <v>4</v>
+      </c>
+      <c r="I5" s="48">
+        <v>41364</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A6" s="37" t="s">

</xml_diff>